<commit_message>
Remove Space after Television in Yield
</commit_message>
<xml_diff>
--- a/data/DataPBAS.xlsx
+++ b/data/DataPBAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikew\Desktop\University\TilburgUniversity\Master\professional_business_analytics_skills\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0C5395-9791-4AE7-9361-35256C8D01ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5032245-924F-4BF1-B1A1-AF890AA0ED49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9F4E300F-392D-41AA-9513-FB2EB37B5714}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{9F4E300F-392D-41AA-9513-FB2EB37B5714}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductSize" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>VGA</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>million USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Television </t>
   </si>
   <si>
     <t>Max capacity</t>
@@ -561,13 +558,13 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -930,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6573A45-A7E9-4D9E-9E5C-16C5E6687B73}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1724,10 +1721,10 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -1902,10 +1899,10 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -1982,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED897D7E-47F5-4242-AA61-4DF3F8F0F250}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1993,13 +1990,13 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1">
         <v>2003</v>
@@ -2154,7 +2151,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1">
         <v>0.3</v>
@@ -2217,21 +2214,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
       <c r="C2">
         <v>60000</v>
@@ -2239,10 +2236,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
       </c>
       <c r="C3" s="1">
         <v>0.05</v>
@@ -2250,10 +2247,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1">
         <v>0.04</v>
@@ -2261,10 +2258,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>0.1</v>
@@ -2272,10 +2269,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -2283,10 +2280,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
       </c>
       <c r="C7">
         <v>1.5</v>
@@ -2294,10 +2291,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
       </c>
       <c r="C8">
         <v>1.8</v>
@@ -2305,10 +2302,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
         <v>0.25</v>
@@ -2316,10 +2313,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
       </c>
       <c r="C10">
         <v>45</v>
@@ -2327,10 +2324,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>45</v>
@@ -2338,10 +2335,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>30</v>

</xml_diff>